<commit_message>
Começando interação com o banco de dados pensando nas batidas de ponto
</commit_message>
<xml_diff>
--- a/PontoEletrônico.xlsx
+++ b/PontoEletrônico.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="29">
   <si>
     <t xml:space="preserve">DATA</t>
   </si>
@@ -92,6 +92,21 @@
   </si>
   <si>
     <t>19:00:00</t>
+  </si>
+  <si>
+    <t>17/10/2023</t>
+  </si>
+  <si>
+    <t>15:28:20</t>
+  </si>
+  <si>
+    <t>15:28:25</t>
+  </si>
+  <si>
+    <t>15:28:29</t>
+  </si>
+  <si>
+    <t>15:28:30</t>
   </si>
 </sst>
 </file>
@@ -196,7 +211,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
@@ -343,6 +358,23 @@
         <v>19</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="E9" t="s" s="0">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>